<commit_message>
modify doc for specification change
</commit_message>
<xml_diff>
--- a/calc/doc/BasicDesignDoc.xlsx
+++ b/calc/doc/BasicDesignDoc.xlsx
@@ -332,8 +332,8 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>「計算結果は○○です」と出力。</t>
-    <rPh sb="12" eb="14">
+    <t>「計算結果は○○です。」と出力。</t>
+    <rPh sb="13" eb="15">
       <t>シュツリョク</t>
     </rPh>
     <phoneticPr fontId="1"/>

</xml_diff>